<commit_message>
feat: support combined desglose 'Turno + Máquina' and make tests runnable; add smoke import helper; sys.path fix for Streamlit Cloud
</commit_message>
<xml_diff>
--- a/REFERENCIAS/Claves_de_Rechazo-GPT.xlsx
+++ b/REFERENCIAS/Claves_de_Rechazo-GPT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="145">
   <si>
     <t>Clave</t>
   </si>
@@ -446,6 +446,9 @@
   </si>
   <si>
     <t>Categoria</t>
+  </si>
+  <si>
+    <t>OTRO</t>
   </si>
 </sst>
 </file>
@@ -770,7 +773,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -900,6 +903,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -945,9 +959,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1292,13 +1307,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="84.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2008,10 +2024,12 @@
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>